<commit_message>
Moved the "test-model-library" to `dev` folder. This test is nice to check the behavior in the package in differently complex tasks, but is too heavy for a unit test.
</commit_message>
<xml_diff>
--- a/inst/extdata/Clarithromycin_Profiles.xlsx
+++ b/inst/extdata/Clarithromycin_Profiles.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\OSPSuite.ParameterIdentification\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994EC193-431A-4176-BC97-B3C5B4776FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424F8FCA-11CB-4B75-AEA0-99D12C924B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PO250MD" sheetId="2" r:id="rId1"/>
     <sheet name="PO250" sheetId="3" r:id="rId2"/>
     <sheet name="PO500MD" sheetId="4" r:id="rId3"/>
     <sheet name="PO500" sheetId="5" r:id="rId4"/>
-    <sheet name="IV250SD" sheetId="6" r:id="rId5"/>
+    <sheet name="IV250" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1335,7 +1335,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>